<commit_message>
Sheamin created new figures (images in source folder) and edited data files
</commit_message>
<xml_diff>
--- a/data/All Data.xlsx
+++ b/data/All Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dears\Documents\info201\project-group-2-section-ae\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D77513F-5F27-4868-B49F-78FE2E8556D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A9AE615-9EE6-4E50-9AE6-4B99028EEA25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="17472" windowHeight="10272" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -234,7 +234,7 @@
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -269,10 +269,6 @@
     </xf>
     <xf numFmtId="4" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="11">
@@ -567,7 +563,7 @@
   <dimension ref="A1:X9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="X2" sqref="X2"/>
+      <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -621,10 +617,10 @@
       <c r="U1" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="V1" s="13" t="s">
+      <c r="V1" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="W1" s="13" t="s">
+      <c r="W1" s="7" t="s">
         <v>47</v>
       </c>
       <c r="X1" t="s">
@@ -680,7 +676,7 @@
       <c r="T2" s="5">
         <v>2213</v>
       </c>
-      <c r="U2" s="14"/>
+      <c r="U2" s="9"/>
       <c r="V2" s="4" t="s">
         <v>38</v>
       </c>

</xml_diff>